<commit_message>
Graph part done and added with a few errors.
</commit_message>
<xml_diff>
--- a/R_Shiny/Data/Employee_Data_Multiple.xlsx
+++ b/R_Shiny/Data/Employee_Data_Multiple.xlsx
@@ -5,36 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Adesh FAU HIS\SEM 3\HIS Project (ML)\Data Pre-Processing HIS Project Andersson\HIS_Project_Shiny\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\HIS-project\HIS-Project\R_Shiny\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F767496-F220-4DF8-B180-1C88AA5104C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C2D6E8-2E25-49D6-B577-B5906EAF5057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="1" r:id="rId1"/>
     <sheet name="Data2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="328">
   <si>
     <t>Age</t>
   </si>
@@ -490,16 +477,550 @@
   </si>
   <si>
     <t>Adesh</t>
+  </si>
+  <si>
+    <t>Sa1lary</t>
+  </si>
+  <si>
+    <t>Sa222lary</t>
+  </si>
+  <si>
+    <t>YP+OE</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>1.1.1996</t>
+  </si>
+  <si>
+    <t>1.1.1997</t>
+  </si>
+  <si>
+    <t>1.1.1998</t>
+  </si>
+  <si>
+    <t>1.1.1999</t>
+  </si>
+  <si>
+    <t>1.1.2000</t>
+  </si>
+  <si>
+    <t>1.1.2001</t>
+  </si>
+  <si>
+    <t>1.1.2002</t>
+  </si>
+  <si>
+    <t>1.1.2003</t>
+  </si>
+  <si>
+    <t>1.1.2004</t>
+  </si>
+  <si>
+    <t>1.1.2005</t>
+  </si>
+  <si>
+    <t>1.1.2006</t>
+  </si>
+  <si>
+    <t>1.1.2007</t>
+  </si>
+  <si>
+    <t>1.1.2008</t>
+  </si>
+  <si>
+    <t>1.1.2009</t>
+  </si>
+  <si>
+    <t>1.1.2010</t>
+  </si>
+  <si>
+    <t>1.1.2011</t>
+  </si>
+  <si>
+    <t>1.1.2012</t>
+  </si>
+  <si>
+    <t>1.1.2013</t>
+  </si>
+  <si>
+    <t>1.1.2014</t>
+  </si>
+  <si>
+    <t>1.1.2015</t>
+  </si>
+  <si>
+    <t>1.1.2016</t>
+  </si>
+  <si>
+    <t>1.1.2017</t>
+  </si>
+  <si>
+    <t>1.1.2018</t>
+  </si>
+  <si>
+    <t>1.1.2019</t>
+  </si>
+  <si>
+    <t>1.1.2020</t>
+  </si>
+  <si>
+    <t>1.1.2021</t>
+  </si>
+  <si>
+    <t>1.1.2022</t>
+  </si>
+  <si>
+    <t>1.1.2023</t>
+  </si>
+  <si>
+    <t>1.1.2024</t>
+  </si>
+  <si>
+    <t>1.1.2025</t>
+  </si>
+  <si>
+    <t>1.1.2026</t>
+  </si>
+  <si>
+    <t>1.1.2027</t>
+  </si>
+  <si>
+    <t>1.1.2028</t>
+  </si>
+  <si>
+    <t>1.1.2029</t>
+  </si>
+  <si>
+    <t>1.1.2030</t>
+  </si>
+  <si>
+    <t>1.1.2031</t>
+  </si>
+  <si>
+    <t>1.1.2032</t>
+  </si>
+  <si>
+    <t>1.1.2033</t>
+  </si>
+  <si>
+    <t>1.1.2034</t>
+  </si>
+  <si>
+    <t>1.1.2035</t>
+  </si>
+  <si>
+    <t>1.1.2036</t>
+  </si>
+  <si>
+    <t>1.1.2037</t>
+  </si>
+  <si>
+    <t>1.1.2038</t>
+  </si>
+  <si>
+    <t>1.1.2039</t>
+  </si>
+  <si>
+    <t>1.1.2040</t>
+  </si>
+  <si>
+    <t>1.1.2041</t>
+  </si>
+  <si>
+    <t>1.1.2042</t>
+  </si>
+  <si>
+    <t>1.1.2043</t>
+  </si>
+  <si>
+    <t>1.1.2044</t>
+  </si>
+  <si>
+    <t>1.1.2045</t>
+  </si>
+  <si>
+    <t>1.1.2046</t>
+  </si>
+  <si>
+    <t>1.1.2047</t>
+  </si>
+  <si>
+    <t>1.1.2048</t>
+  </si>
+  <si>
+    <t>1.1.2049</t>
+  </si>
+  <si>
+    <t>1.1.2050</t>
+  </si>
+  <si>
+    <t>1.1.2051</t>
+  </si>
+  <si>
+    <t>1.1.2052</t>
+  </si>
+  <si>
+    <t>1.1.2053</t>
+  </si>
+  <si>
+    <t>1.1.2054</t>
+  </si>
+  <si>
+    <t>1.1.2055</t>
+  </si>
+  <si>
+    <t>1.1.2056</t>
+  </si>
+  <si>
+    <t>1.1.2057</t>
+  </si>
+  <si>
+    <t>1.1.2058</t>
+  </si>
+  <si>
+    <t>1.1.2059</t>
+  </si>
+  <si>
+    <t>1.1.2060</t>
+  </si>
+  <si>
+    <t>1.1.2061</t>
+  </si>
+  <si>
+    <t>1.1.2062</t>
+  </si>
+  <si>
+    <t>1.1.2063</t>
+  </si>
+  <si>
+    <t>1.1.2064</t>
+  </si>
+  <si>
+    <t>1.1.2065</t>
+  </si>
+  <si>
+    <t>1.1.2066</t>
+  </si>
+  <si>
+    <t>1.1.2067</t>
+  </si>
+  <si>
+    <t>1.1.2068</t>
+  </si>
+  <si>
+    <t>1.1.2069</t>
+  </si>
+  <si>
+    <t>1.1.2070</t>
+  </si>
+  <si>
+    <t>1.1.2071</t>
+  </si>
+  <si>
+    <t>1.1.2072</t>
+  </si>
+  <si>
+    <t>1.1.2073</t>
+  </si>
+  <si>
+    <t>1.1.2074</t>
+  </si>
+  <si>
+    <t>1.1.2075</t>
+  </si>
+  <si>
+    <t>1.1.2076</t>
+  </si>
+  <si>
+    <t>1.1.2077</t>
+  </si>
+  <si>
+    <t>1.1.2078</t>
+  </si>
+  <si>
+    <t>1.1.2079</t>
+  </si>
+  <si>
+    <t>1.1.2080</t>
+  </si>
+  <si>
+    <t>1.1.2081</t>
+  </si>
+  <si>
+    <t>1.1.2082</t>
+  </si>
+  <si>
+    <t>1.1.2083</t>
+  </si>
+  <si>
+    <t>1.1.2084</t>
+  </si>
+  <si>
+    <t>1.1.2085</t>
+  </si>
+  <si>
+    <t>1.1.2086</t>
+  </si>
+  <si>
+    <t>1.1.2087</t>
+  </si>
+  <si>
+    <t>1.1.2088</t>
+  </si>
+  <si>
+    <t>1.1.2089</t>
+  </si>
+  <si>
+    <t>1.1.2090</t>
+  </si>
+  <si>
+    <t>1.1.2091</t>
+  </si>
+  <si>
+    <t>1.1.2092</t>
+  </si>
+  <si>
+    <t>1.1.2093</t>
+  </si>
+  <si>
+    <t>1.1.2094</t>
+  </si>
+  <si>
+    <t>1.1.2095</t>
+  </si>
+  <si>
+    <t>1.1.2096</t>
+  </si>
+  <si>
+    <t>1.1.2097</t>
+  </si>
+  <si>
+    <t>1.1.2098</t>
+  </si>
+  <si>
+    <t>1.1.2099</t>
+  </si>
+  <si>
+    <t>1.1.2100</t>
+  </si>
+  <si>
+    <t>1.1.2101</t>
+  </si>
+  <si>
+    <t>1.1.2102</t>
+  </si>
+  <si>
+    <t>1.1.2103</t>
+  </si>
+  <si>
+    <t>1.1.2104</t>
+  </si>
+  <si>
+    <t>1.1.2105</t>
+  </si>
+  <si>
+    <t>1.1.2106</t>
+  </si>
+  <si>
+    <t>1.1.2107</t>
+  </si>
+  <si>
+    <t>1.1.2108</t>
+  </si>
+  <si>
+    <t>1.1.2109</t>
+  </si>
+  <si>
+    <t>1.1.2110</t>
+  </si>
+  <si>
+    <t>1.1.2111</t>
+  </si>
+  <si>
+    <t>1.1.2112</t>
+  </si>
+  <si>
+    <t>1.1.2113</t>
+  </si>
+  <si>
+    <t>1.1.2114</t>
+  </si>
+  <si>
+    <t>1.1.2115</t>
+  </si>
+  <si>
+    <t>1.1.2116</t>
+  </si>
+  <si>
+    <t>1.1.2117</t>
+  </si>
+  <si>
+    <t>1.1.2118</t>
+  </si>
+  <si>
+    <t>1.1.2119</t>
+  </si>
+  <si>
+    <t>1.1.2120</t>
+  </si>
+  <si>
+    <t>1.1.2121</t>
+  </si>
+  <si>
+    <t>1.1.2122</t>
+  </si>
+  <si>
+    <t>1.1.2123</t>
+  </si>
+  <si>
+    <t>1.1.2124</t>
+  </si>
+  <si>
+    <t>1.1.2125</t>
+  </si>
+  <si>
+    <t>1.1.2126</t>
+  </si>
+  <si>
+    <t>1.1.2127</t>
+  </si>
+  <si>
+    <t>1.1.2128</t>
+  </si>
+  <si>
+    <t>1.1.2129</t>
+  </si>
+  <si>
+    <t>1.1.2130</t>
+  </si>
+  <si>
+    <t>1.1.2131</t>
+  </si>
+  <si>
+    <t>1.1.2132</t>
+  </si>
+  <si>
+    <t>1.1.2133</t>
+  </si>
+  <si>
+    <t>1.1.2134</t>
+  </si>
+  <si>
+    <t>1.1.2135</t>
+  </si>
+  <si>
+    <t>1.1.2136</t>
+  </si>
+  <si>
+    <t>1.1.2137</t>
+  </si>
+  <si>
+    <t>1.1.2138</t>
+  </si>
+  <si>
+    <t>1.1.2139</t>
+  </si>
+  <si>
+    <t>1.1.2140</t>
+  </si>
+  <si>
+    <t>1.1.2141</t>
+  </si>
+  <si>
+    <t>1.1.2142</t>
+  </si>
+  <si>
+    <t>1.1.2143</t>
+  </si>
+  <si>
+    <t>1.1.2144</t>
+  </si>
+  <si>
+    <t>1.1.2145</t>
+  </si>
+  <si>
+    <t>1.1.2146</t>
+  </si>
+  <si>
+    <t>1.1.2147</t>
+  </si>
+  <si>
+    <t>1.1.2148</t>
+  </si>
+  <si>
+    <t>1.1.2149</t>
+  </si>
+  <si>
+    <t>1.1.2150</t>
+  </si>
+  <si>
+    <t>1.1.2151</t>
+  </si>
+  <si>
+    <t>1.1.2152</t>
+  </si>
+  <si>
+    <t>1.1.2153</t>
+  </si>
+  <si>
+    <t>1.1.2154</t>
+  </si>
+  <si>
+    <t>1.1.2155</t>
+  </si>
+  <si>
+    <t>1.1.2156</t>
+  </si>
+  <si>
+    <t>1.1.2157</t>
+  </si>
+  <si>
+    <t>1.1.2158</t>
+  </si>
+  <si>
+    <t>1.1.2159</t>
+  </si>
+  <si>
+    <t>1.1.2160</t>
+  </si>
+  <si>
+    <t>1.1.2161</t>
+  </si>
+  <si>
+    <t>1.1.2162</t>
+  </si>
+  <si>
+    <t>1.1.2163</t>
+  </si>
+  <si>
+    <t>1.1.2164</t>
+  </si>
+  <si>
+    <t>1.1.2165</t>
+  </si>
+  <si>
+    <t>1.1.2166</t>
+  </si>
+  <si>
+    <t>1.1.2167</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1019,23 +1540,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F173"/>
+  <dimension ref="A1:J173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K170" sqref="K170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1054,8 +1575,20 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>27</v>
       </c>
@@ -1071,8 +1604,17 @@
       <c r="F2">
         <v>9762362</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2">
+        <v>9762362</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>28</v>
       </c>
@@ -1091,8 +1633,17 @@
       <c r="F3">
         <v>65000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3">
+        <v>65000000</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>45</v>
       </c>
@@ -1111,8 +1662,20 @@
       <c r="F4">
         <v>150012312300</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>150012312300</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -1125,8 +1688,20 @@
       <c r="F5">
         <v>60000</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>60000</v>
+      </c>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -1139,8 +1714,20 @@
       <c r="F6">
         <v>2000003332</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>2000003332</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1156,8 +1743,20 @@
       <c r="F7">
         <v>55000</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>55000</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -1173,8 +1772,20 @@
       <c r="F8">
         <v>12000012313</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>12000012313</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1190,8 +1801,20 @@
       <c r="F9">
         <v>80000123123</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>80000123123</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -1204,8 +1827,20 @@
       <c r="F10">
         <v>45000</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>45000</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11" t="s">
         <v>6</v>
       </c>
@@ -1218,8 +1853,20 @@
       <c r="F11">
         <v>110000</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>110000</v>
+      </c>
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -1235,8 +1882,20 @@
       <c r="F12">
         <v>75000121</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>75000121</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13" t="s">
         <v>9</v>
       </c>
@@ -1252,8 +1911,20 @@
       <c r="F13">
         <v>140000</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>140000</v>
+      </c>
+      <c r="I13">
+        <v>18</v>
+      </c>
+      <c r="J13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -1269,8 +1940,20 @@
       <c r="F14">
         <v>65000</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>65000</v>
+      </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -1283,8 +1966,20 @@
       <c r="F15">
         <v>130000123123</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>18</v>
+      </c>
+      <c r="H15">
+        <v>130000123123</v>
+      </c>
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>27</v>
       </c>
@@ -1300,8 +1995,20 @@
       <c r="F16">
         <v>40000</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="H16">
+        <v>40000</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>44</v>
       </c>
@@ -1320,8 +2027,20 @@
       <c r="F17">
         <v>125000</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>14</v>
+      </c>
+      <c r="H17">
+        <v>125000</v>
+      </c>
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>33</v>
       </c>
@@ -1340,8 +2059,20 @@
       <c r="F18">
         <v>90000</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>90000</v>
+      </c>
+      <c r="I18">
+        <v>7</v>
+      </c>
+      <c r="J18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>39</v>
       </c>
@@ -1360,8 +2091,20 @@
       <c r="F19">
         <v>115000123213</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>16</v>
+      </c>
+      <c r="H19">
+        <v>115000123213</v>
+      </c>
+      <c r="I19">
+        <v>12</v>
+      </c>
+      <c r="J19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>25</v>
       </c>
@@ -1380,8 +2123,20 @@
       <c r="F20">
         <v>35000</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>35000</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>51</v>
       </c>
@@ -1400,8 +2155,20 @@
       <c r="F21">
         <v>180000</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>12</v>
+      </c>
+      <c r="H21">
+        <v>180000</v>
+      </c>
+      <c r="I21">
+        <v>22</v>
+      </c>
+      <c r="J21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>34</v>
       </c>
@@ -1417,8 +2184,20 @@
       <c r="F22">
         <v>80000</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>80000</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>47</v>
       </c>
@@ -1434,8 +2213,20 @@
       <c r="F23">
         <v>190000</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>22</v>
+      </c>
+      <c r="H23">
+        <v>190000</v>
+      </c>
+      <c r="I23">
+        <v>19</v>
+      </c>
+      <c r="J23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>30</v>
       </c>
@@ -1451,8 +2242,20 @@
       <c r="F24">
         <v>50000</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>50000</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>36</v>
       </c>
@@ -1471,8 +2274,20 @@
       <c r="F25">
         <v>60000123123</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>19</v>
+      </c>
+      <c r="H25">
+        <v>60000123123</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+      <c r="J25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>41</v>
       </c>
@@ -1491,8 +2306,20 @@
       <c r="F26">
         <v>140000</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>140000</v>
+      </c>
+      <c r="I26">
+        <v>13</v>
+      </c>
+      <c r="J26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>28</v>
       </c>
@@ -1511,8 +2338,20 @@
       <c r="F27">
         <v>45000</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>9</v>
+      </c>
+      <c r="H27">
+        <v>45000</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+      <c r="J27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>37</v>
       </c>
@@ -1531,8 +2370,20 @@
       <c r="F28">
         <v>110000</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>13</v>
+      </c>
+      <c r="H28">
+        <v>110000</v>
+      </c>
+      <c r="I28">
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>24</v>
       </c>
@@ -1551,8 +2402,20 @@
       <c r="F29">
         <v>40000</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>40000</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>43</v>
       </c>
@@ -1571,8 +2434,20 @@
       <c r="F30">
         <v>140000</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>11</v>
+      </c>
+      <c r="H30">
+        <v>140000</v>
+      </c>
+      <c r="I30">
+        <v>15</v>
+      </c>
+      <c r="J30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>33</v>
       </c>
@@ -1591,8 +2466,20 @@
       <c r="F31">
         <v>90000</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>90000</v>
+      </c>
+      <c r="I31">
+        <v>6</v>
+      </c>
+      <c r="J31" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>50</v>
       </c>
@@ -1611,8 +2498,20 @@
       <c r="F32">
         <v>250000</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>15</v>
+      </c>
+      <c r="H32">
+        <v>250000</v>
+      </c>
+      <c r="I32">
+        <v>25</v>
+      </c>
+      <c r="J32" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1631,8 +2530,20 @@
       <c r="F33">
         <v>55000</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>6</v>
+      </c>
+      <c r="H33">
+        <v>55000</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+      <c r="J33" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>29</v>
       </c>
@@ -1651,8 +2562,20 @@
       <c r="F34">
         <v>75000</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>25</v>
+      </c>
+      <c r="H34">
+        <v>75000</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="J34" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>39</v>
       </c>
@@ -1671,8 +2594,20 @@
       <c r="F35">
         <v>65000</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <v>65000</v>
+      </c>
+      <c r="I35">
+        <v>10</v>
+      </c>
+      <c r="J35" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>46</v>
       </c>
@@ -1691,8 +2626,20 @@
       <c r="F36">
         <v>170000</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>170000</v>
+      </c>
+      <c r="I36">
+        <v>20</v>
+      </c>
+      <c r="J36" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>27</v>
       </c>
@@ -1711,8 +2658,20 @@
       <c r="F37">
         <v>450002222123</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>10</v>
+      </c>
+      <c r="H37">
+        <v>450002222123</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>35</v>
       </c>
@@ -1731,8 +2690,20 @@
       <c r="F38">
         <v>60000</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>20</v>
+      </c>
+      <c r="H38">
+        <v>60000</v>
+      </c>
+      <c r="I38">
+        <v>7</v>
+      </c>
+      <c r="J38" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>42</v>
       </c>
@@ -1751,8 +2722,20 @@
       <c r="F39">
         <v>115000</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>115000</v>
+      </c>
+      <c r="I39">
+        <v>14</v>
+      </c>
+      <c r="J39" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>26</v>
       </c>
@@ -1771,8 +2754,20 @@
       <c r="F40">
         <v>40000123214</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="H40">
+        <v>40000123214</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>49</v>
       </c>
@@ -1791,8 +2786,20 @@
       <c r="F41">
         <v>160000</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <v>14</v>
+      </c>
+      <c r="H41">
+        <v>160000</v>
+      </c>
+      <c r="I41">
+        <v>21</v>
+      </c>
+      <c r="J41" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>34</v>
       </c>
@@ -1811,8 +2818,20 @@
       <c r="F42">
         <v>80000</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>80000</v>
+      </c>
+      <c r="I42">
+        <v>5</v>
+      </c>
+      <c r="J42" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>48</v>
       </c>
@@ -1831,8 +2850,20 @@
       <c r="F43">
         <v>190000</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <v>21</v>
+      </c>
+      <c r="H43">
+        <v>190000</v>
+      </c>
+      <c r="I43">
+        <v>18</v>
+      </c>
+      <c r="J43" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>30</v>
       </c>
@@ -1851,8 +2882,20 @@
       <c r="F44">
         <v>60000</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <v>5</v>
+      </c>
+      <c r="H44">
+        <v>60000</v>
+      </c>
+      <c r="I44">
+        <v>3</v>
+      </c>
+      <c r="J44" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>36</v>
       </c>
@@ -1871,8 +2914,20 @@
       <c r="F45">
         <v>45000</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>18</v>
+      </c>
+      <c r="H45">
+        <v>45000</v>
+      </c>
+      <c r="I45">
+        <v>8</v>
+      </c>
+      <c r="J45" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>41</v>
       </c>
@@ -1891,8 +2946,20 @@
       <c r="F46">
         <v>130000134143</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>130000134143</v>
+      </c>
+      <c r="I46">
+        <v>13</v>
+      </c>
+      <c r="J46" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>28</v>
       </c>
@@ -1911,8 +2978,20 @@
       <c r="F47">
         <v>40000</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>8</v>
+      </c>
+      <c r="H47">
+        <v>40000</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>32</v>
       </c>
@@ -1931,8 +3010,20 @@
       <c r="F48">
         <v>75000</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <v>13</v>
+      </c>
+      <c r="H48">
+        <v>75000</v>
+      </c>
+      <c r="I48">
+        <v>5</v>
+      </c>
+      <c r="J48" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>45</v>
       </c>
@@ -1951,8 +3042,20 @@
       <c r="F49">
         <v>180000</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <v>2</v>
+      </c>
+      <c r="H49">
+        <v>180000</v>
+      </c>
+      <c r="I49">
+        <v>16</v>
+      </c>
+      <c r="J49" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>38</v>
       </c>
@@ -1971,8 +3074,20 @@
       <c r="F50">
         <v>120000</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <v>120000</v>
+      </c>
+      <c r="I50">
+        <v>11</v>
+      </c>
+      <c r="J50" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>25</v>
       </c>
@@ -1991,8 +3106,20 @@
       <c r="F51">
         <v>35000</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <v>16</v>
+      </c>
+      <c r="H51">
+        <v>35000</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2011,8 +3138,20 @@
       <c r="F52">
         <v>130000</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <v>11</v>
+      </c>
+      <c r="H52">
+        <v>130000</v>
+      </c>
+      <c r="I52">
+        <v>22</v>
+      </c>
+      <c r="J52" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>33</v>
       </c>
@@ -2031,8 +3170,20 @@
       <c r="F53">
         <v>85000</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>85000</v>
+      </c>
+      <c r="I53">
+        <v>7</v>
+      </c>
+      <c r="J53" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>40</v>
       </c>
@@ -2051,8 +3202,20 @@
       <c r="F54">
         <v>1234123</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54">
+        <v>22</v>
+      </c>
+      <c r="H54">
+        <v>1234123</v>
+      </c>
+      <c r="I54">
+        <v>12</v>
+      </c>
+      <c r="J54" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>47</v>
       </c>
@@ -2071,8 +3234,20 @@
       <c r="F55">
         <v>200000</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55">
+        <v>7</v>
+      </c>
+      <c r="H55">
+        <v>200000</v>
+      </c>
+      <c r="I55">
+        <v>19</v>
+      </c>
+      <c r="J55" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>29</v>
       </c>
@@ -2091,8 +3266,20 @@
       <c r="F56">
         <v>50000</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56">
+        <v>12</v>
+      </c>
+      <c r="H56">
+        <v>50000</v>
+      </c>
+      <c r="I56">
+        <v>3</v>
+      </c>
+      <c r="J56" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>36</v>
       </c>
@@ -2111,8 +3298,20 @@
       <c r="F57">
         <v>95000</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57">
+        <v>19</v>
+      </c>
+      <c r="H57">
+        <v>95000</v>
+      </c>
+      <c r="I57">
+        <v>9</v>
+      </c>
+      <c r="J57" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>27</v>
       </c>
@@ -2131,8 +3330,20 @@
       <c r="F58">
         <v>65000</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <v>65000</v>
+      </c>
+      <c r="I58">
+        <v>2</v>
+      </c>
+      <c r="J58" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="B59" t="s">
         <v>6</v>
       </c>
@@ -2148,8 +3359,20 @@
       <c r="F59">
         <v>140000</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59">
+        <v>9</v>
+      </c>
+      <c r="H59">
+        <v>140000</v>
+      </c>
+      <c r="I59">
+        <v>17</v>
+      </c>
+      <c r="J59" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="B60" t="s">
         <v>9</v>
       </c>
@@ -2165,8 +3388,20 @@
       <c r="F60">
         <v>55000</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60">
+        <v>2</v>
+      </c>
+      <c r="H60">
+        <v>55000</v>
+      </c>
+      <c r="I60">
+        <v>4</v>
+      </c>
+      <c r="J60" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="B61" t="s">
         <v>6</v>
       </c>
@@ -2182,8 +3417,20 @@
       <c r="F61">
         <v>105000</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61">
+        <v>17</v>
+      </c>
+      <c r="H61">
+        <v>105000</v>
+      </c>
+      <c r="I61">
+        <v>7</v>
+      </c>
+      <c r="J61" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="B62" t="s">
         <v>9</v>
       </c>
@@ -2199,8 +3446,20 @@
       <c r="F62">
         <v>170000</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62">
+        <v>4</v>
+      </c>
+      <c r="H62">
+        <v>170000</v>
+      </c>
+      <c r="I62">
+        <v>23</v>
+      </c>
+      <c r="J62" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="B63" t="s">
         <v>6</v>
       </c>
@@ -2216,8 +3475,20 @@
       <c r="F63">
         <v>50000</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63">
+        <v>7</v>
+      </c>
+      <c r="H63">
+        <v>50000</v>
+      </c>
+      <c r="I63">
+        <v>3</v>
+      </c>
+      <c r="J63" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="B64" t="s">
         <v>9</v>
       </c>
@@ -2233,8 +3504,20 @@
       <c r="F64">
         <v>80000</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64">
+        <v>23</v>
+      </c>
+      <c r="H64">
+        <v>80000</v>
+      </c>
+      <c r="I64">
+        <v>12</v>
+      </c>
+      <c r="J64" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="B65" t="s">
         <v>6</v>
       </c>
@@ -2250,8 +3533,20 @@
       <c r="F65">
         <v>180000</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65">
+        <v>3</v>
+      </c>
+      <c r="H65">
+        <v>180000</v>
+      </c>
+      <c r="I65">
+        <v>21</v>
+      </c>
+      <c r="J65" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="B66" t="s">
         <v>6</v>
       </c>
@@ -2267,8 +3562,20 @@
       <c r="F66">
         <v>35000</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66">
+        <v>12</v>
+      </c>
+      <c r="H66">
+        <v>35000</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="B67" t="s">
         <v>9</v>
       </c>
@@ -2284,8 +3591,20 @@
       <c r="F67">
         <v>90000</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67">
+        <v>21</v>
+      </c>
+      <c r="H67">
+        <v>90000</v>
+      </c>
+      <c r="I67">
+        <v>10</v>
+      </c>
+      <c r="J67" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>46</v>
       </c>
@@ -2304,8 +3623,20 @@
       <c r="F68">
         <v>120000</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>120000</v>
+      </c>
+      <c r="I68">
+        <v>19</v>
+      </c>
+      <c r="J68" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>31</v>
       </c>
@@ -2324,8 +3655,20 @@
       <c r="F69">
         <v>45000</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69">
+        <v>10</v>
+      </c>
+      <c r="H69">
+        <v>45000</v>
+      </c>
+      <c r="I69">
+        <v>5</v>
+      </c>
+      <c r="J69" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>34</v>
       </c>
@@ -2344,8 +3687,20 @@
       <c r="F70">
         <v>90000</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70">
+        <v>19</v>
+      </c>
+      <c r="H70">
+        <v>90000</v>
+      </c>
+      <c r="I70">
+        <v>8</v>
+      </c>
+      <c r="J70" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>49</v>
       </c>
@@ -2364,8 +3719,20 @@
       <c r="F71">
         <v>150000</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71">
+        <v>5</v>
+      </c>
+      <c r="H71">
+        <v>150000</v>
+      </c>
+      <c r="I71">
+        <v>18</v>
+      </c>
+      <c r="J71" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>33</v>
       </c>
@@ -2384,8 +3751,20 @@
       <c r="F72">
         <v>65000</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72">
+        <v>8</v>
+      </c>
+      <c r="H72">
+        <v>65000</v>
+      </c>
+      <c r="I72">
+        <v>6</v>
+      </c>
+      <c r="J72" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>39</v>
       </c>
@@ -2404,8 +3783,20 @@
       <c r="F73">
         <v>70000</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73">
+        <v>18</v>
+      </c>
+      <c r="H73">
+        <v>70000</v>
+      </c>
+      <c r="I73">
+        <v>11</v>
+      </c>
+      <c r="J73" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>45</v>
       </c>
@@ -2424,8 +3815,20 @@
       <c r="F74">
         <v>190000</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74">
+        <v>6</v>
+      </c>
+      <c r="H74">
+        <v>190000</v>
+      </c>
+      <c r="I74">
+        <v>16</v>
+      </c>
+      <c r="J74" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>28</v>
       </c>
@@ -2444,8 +3847,20 @@
       <c r="F75">
         <v>40000</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75">
+        <v>11</v>
+      </c>
+      <c r="H75">
+        <v>40000</v>
+      </c>
+      <c r="I75">
+        <v>2</v>
+      </c>
+      <c r="J75" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>42</v>
       </c>
@@ -2464,8 +3879,20 @@
       <c r="F76">
         <v>120000</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76">
+        <v>16</v>
+      </c>
+      <c r="H76">
+        <v>120000</v>
+      </c>
+      <c r="I76">
+        <v>14</v>
+      </c>
+      <c r="J76" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>37</v>
       </c>
@@ -2484,8 +3911,20 @@
       <c r="F77">
         <v>95000</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77">
+        <v>2</v>
+      </c>
+      <c r="H77">
+        <v>95000</v>
+      </c>
+      <c r="I77">
+        <v>10</v>
+      </c>
+      <c r="J77" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>50</v>
       </c>
@@ -2504,8 +3943,20 @@
       <c r="F78">
         <v>160000</v>
       </c>
-    </row>
-    <row r="79" spans="1:6">
+      <c r="G78">
+        <v>14</v>
+      </c>
+      <c r="H78">
+        <v>160000</v>
+      </c>
+      <c r="I78">
+        <v>22</v>
+      </c>
+      <c r="J78" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>32</v>
       </c>
@@ -2524,8 +3975,20 @@
       <c r="F79">
         <v>100000</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79">
+        <v>10</v>
+      </c>
+      <c r="H79">
+        <v>100000</v>
+      </c>
+      <c r="I79">
+        <v>6</v>
+      </c>
+      <c r="J79" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>48</v>
       </c>
@@ -2544,8 +4007,20 @@
       <c r="F80">
         <v>180000</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80">
+        <v>22</v>
+      </c>
+      <c r="H80">
+        <v>180000</v>
+      </c>
+      <c r="I80">
+        <v>20</v>
+      </c>
+      <c r="J80" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>30</v>
       </c>
@@ -2564,8 +4039,20 @@
       <c r="F81">
         <v>55000</v>
       </c>
-    </row>
-    <row r="82" spans="1:6">
+      <c r="G81">
+        <v>6</v>
+      </c>
+      <c r="H81">
+        <v>55000</v>
+      </c>
+      <c r="I81">
+        <v>3</v>
+      </c>
+      <c r="J81" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>36</v>
       </c>
@@ -2584,8 +4071,20 @@
       <c r="F82">
         <v>70000</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="G82">
+        <v>20</v>
+      </c>
+      <c r="H82">
+        <v>70000</v>
+      </c>
+      <c r="I82">
+        <v>8</v>
+      </c>
+      <c r="J82" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83">
         <v>41</v>
       </c>
@@ -2604,8 +4103,20 @@
       <c r="F83">
         <v>80000</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="G83">
+        <v>3</v>
+      </c>
+      <c r="H83">
+        <v>80000</v>
+      </c>
+      <c r="I83">
+        <v>13</v>
+      </c>
+      <c r="J83" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84">
         <v>25</v>
       </c>
@@ -2624,8 +4135,20 @@
       <c r="F84">
         <v>30000</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="G84">
+        <v>8</v>
+      </c>
+      <c r="H84">
+        <v>30000</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85">
         <v>52</v>
       </c>
@@ -2644,8 +4167,20 @@
       <c r="F85">
         <v>250000</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="G85">
+        <v>13</v>
+      </c>
+      <c r="H85">
+        <v>250000</v>
+      </c>
+      <c r="I85">
+        <v>24</v>
+      </c>
+      <c r="J85" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86">
         <v>29</v>
       </c>
@@ -2664,8 +4199,20 @@
       <c r="F86">
         <v>40000</v>
       </c>
-    </row>
-    <row r="87" spans="1:6">
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>40000</v>
+      </c>
+      <c r="I86">
+        <v>2</v>
+      </c>
+      <c r="J86" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87">
         <v>34</v>
       </c>
@@ -2684,8 +4231,20 @@
       <c r="F87">
         <v>95000</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="G87">
+        <v>24</v>
+      </c>
+      <c r="H87">
+        <v>95000</v>
+      </c>
+      <c r="I87">
+        <v>10</v>
+      </c>
+      <c r="J87" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88">
         <v>27</v>
       </c>
@@ -2704,8 +4263,20 @@
       <c r="F88">
         <v>45000</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="G88">
+        <v>2</v>
+      </c>
+      <c r="H88">
+        <v>45000</v>
+      </c>
+      <c r="I88">
+        <v>2</v>
+      </c>
+      <c r="J88" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89">
         <v>40</v>
       </c>
@@ -2724,8 +4295,20 @@
       <c r="F89">
         <v>80000</v>
       </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="G89">
+        <v>10</v>
+      </c>
+      <c r="H89">
+        <v>80000</v>
+      </c>
+      <c r="I89">
+        <v>15</v>
+      </c>
+      <c r="J89" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90">
         <v>46</v>
       </c>
@@ -2744,8 +4327,20 @@
       <c r="F90">
         <v>135000</v>
       </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="G90">
+        <v>2</v>
+      </c>
+      <c r="H90">
+        <v>135000</v>
+      </c>
+      <c r="I90">
+        <v>21</v>
+      </c>
+      <c r="J90" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91">
         <v>31</v>
       </c>
@@ -2764,8 +4359,20 @@
       <c r="F91">
         <v>55000</v>
       </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="G91">
+        <v>15</v>
+      </c>
+      <c r="H91">
+        <v>55000</v>
+      </c>
+      <c r="I91">
+        <v>6</v>
+      </c>
+      <c r="J91" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92">
         <v>36</v>
       </c>
@@ -2784,8 +4391,20 @@
       <c r="F92">
         <v>120000</v>
       </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="G92">
+        <v>21</v>
+      </c>
+      <c r="H92">
+        <v>120000</v>
+      </c>
+      <c r="I92">
+        <v>11</v>
+      </c>
+      <c r="J92" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93">
         <v>29</v>
       </c>
@@ -2804,8 +4423,20 @@
       <c r="F93">
         <v>40000</v>
       </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="G93">
+        <v>6</v>
+      </c>
+      <c r="H93">
+        <v>40000</v>
+      </c>
+      <c r="I93">
+        <v>3</v>
+      </c>
+      <c r="J93" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94">
         <v>43</v>
       </c>
@@ -2824,8 +4455,20 @@
       <c r="F94">
         <v>105000</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="G94">
+        <v>11</v>
+      </c>
+      <c r="H94">
+        <v>105000</v>
+      </c>
+      <c r="I94">
+        <v>18</v>
+      </c>
+      <c r="J94" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95">
         <v>52</v>
       </c>
@@ -2844,8 +4487,20 @@
       <c r="F95">
         <v>170000</v>
       </c>
-    </row>
-    <row r="96" spans="1:6">
+      <c r="G95">
+        <v>3</v>
+      </c>
+      <c r="H95">
+        <v>170000</v>
+      </c>
+      <c r="I95">
+        <v>25</v>
+      </c>
+      <c r="J95" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96">
         <v>33</v>
       </c>
@@ -2864,8 +4519,20 @@
       <c r="F96">
         <v>75000</v>
       </c>
-    </row>
-    <row r="97" spans="1:6">
+      <c r="G96">
+        <v>18</v>
+      </c>
+      <c r="H96">
+        <v>75000</v>
+      </c>
+      <c r="I96">
+        <v>7</v>
+      </c>
+      <c r="J96" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97">
         <v>39</v>
       </c>
@@ -2884,8 +4551,20 @@
       <c r="F97">
         <v>65000</v>
       </c>
-    </row>
-    <row r="98" spans="1:6">
+      <c r="G97">
+        <v>25</v>
+      </c>
+      <c r="H97">
+        <v>65000</v>
+      </c>
+      <c r="I97">
+        <v>12</v>
+      </c>
+      <c r="J97" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98">
         <v>47</v>
       </c>
@@ -2904,8 +4583,20 @@
       <c r="F98">
         <v>160000</v>
       </c>
-    </row>
-    <row r="99" spans="1:6">
+      <c r="G98">
+        <v>7</v>
+      </c>
+      <c r="H98">
+        <v>160000</v>
+      </c>
+      <c r="I98">
+        <v>22</v>
+      </c>
+      <c r="J98" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99">
         <v>26</v>
       </c>
@@ -2924,8 +4615,20 @@
       <c r="F99">
         <v>35000</v>
       </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="G99">
+        <v>12</v>
+      </c>
+      <c r="H99">
+        <v>35000</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+      <c r="J99" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100">
         <v>38</v>
       </c>
@@ -2944,8 +4647,20 @@
       <c r="F100">
         <v>90000</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="G100">
+        <v>22</v>
+      </c>
+      <c r="H100">
+        <v>90000</v>
+      </c>
+      <c r="I100">
+        <v>10</v>
+      </c>
+      <c r="J100" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101">
         <v>45</v>
       </c>
@@ -2964,8 +4679,20 @@
       <c r="F101">
         <v>110000</v>
       </c>
-    </row>
-    <row r="102" spans="1:6">
+      <c r="G101">
+        <v>1</v>
+      </c>
+      <c r="H101">
+        <v>110000</v>
+      </c>
+      <c r="I101">
+        <v>20</v>
+      </c>
+      <c r="J101" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102">
         <v>31</v>
       </c>
@@ -2984,8 +4711,20 @@
       <c r="F102">
         <v>45000</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="G102">
+        <v>10</v>
+      </c>
+      <c r="H102">
+        <v>45000</v>
+      </c>
+      <c r="I102">
+        <v>5</v>
+      </c>
+      <c r="J102" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103">
         <v>35</v>
       </c>
@@ -3004,8 +4743,20 @@
       <c r="F103">
         <v>95000</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="G103">
+        <v>20</v>
+      </c>
+      <c r="H103">
+        <v>95000</v>
+      </c>
+      <c r="I103">
+        <v>8</v>
+      </c>
+      <c r="J103" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104">
         <v>49</v>
       </c>
@@ -3024,8 +4775,20 @@
       <c r="F104">
         <v>150000</v>
       </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="G104">
+        <v>5</v>
+      </c>
+      <c r="H104">
+        <v>150000</v>
+      </c>
+      <c r="I104">
+        <v>19</v>
+      </c>
+      <c r="J104" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105">
         <v>33</v>
       </c>
@@ -3044,8 +4807,20 @@
       <c r="F105">
         <v>50000</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="G105">
+        <v>8</v>
+      </c>
+      <c r="H105">
+        <v>50000</v>
+      </c>
+      <c r="I105">
+        <v>5</v>
+      </c>
+      <c r="J105" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106">
         <v>39</v>
       </c>
@@ -3064,8 +4839,20 @@
       <c r="F106">
         <v>80000</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
+      <c r="G106">
+        <v>19</v>
+      </c>
+      <c r="H106">
+        <v>80000</v>
+      </c>
+      <c r="I106">
+        <v>13</v>
+      </c>
+      <c r="J106" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
       <c r="A107">
         <v>44</v>
       </c>
@@ -3084,8 +4871,20 @@
       <c r="F107">
         <v>220000</v>
       </c>
-    </row>
-    <row r="108" spans="1:6">
+      <c r="G107">
+        <v>5</v>
+      </c>
+      <c r="H107">
+        <v>220000</v>
+      </c>
+      <c r="I107">
+        <v>16</v>
+      </c>
+      <c r="J107" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
       <c r="A108">
         <v>30</v>
       </c>
@@ -3104,8 +4903,20 @@
       <c r="F108">
         <v>50000</v>
       </c>
-    </row>
-    <row r="109" spans="1:6">
+      <c r="G108">
+        <v>13</v>
+      </c>
+      <c r="H108">
+        <v>50000</v>
+      </c>
+      <c r="I108">
+        <v>3</v>
+      </c>
+      <c r="J108" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
       <c r="A109">
         <v>36</v>
       </c>
@@ -3124,8 +4935,20 @@
       <c r="F109">
         <v>60000</v>
       </c>
-    </row>
-    <row r="110" spans="1:6">
+      <c r="G109">
+        <v>16</v>
+      </c>
+      <c r="H109">
+        <v>60000</v>
+      </c>
+      <c r="I109">
+        <v>7</v>
+      </c>
+      <c r="J109" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
       <c r="A110">
         <v>41</v>
       </c>
@@ -3144,8 +4967,20 @@
       <c r="F110">
         <v>100000</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
+      <c r="G110">
+        <v>3</v>
+      </c>
+      <c r="H110">
+        <v>100000</v>
+      </c>
+      <c r="I110">
+        <v>14</v>
+      </c>
+      <c r="J110" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
       <c r="A111">
         <v>28</v>
       </c>
@@ -3164,8 +4999,20 @@
       <c r="F111">
         <v>40000</v>
       </c>
-    </row>
-    <row r="112" spans="1:6">
+      <c r="G111">
+        <v>7</v>
+      </c>
+      <c r="H111">
+        <v>40000</v>
+      </c>
+      <c r="I111">
+        <v>2</v>
+      </c>
+      <c r="J111" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112">
         <v>42</v>
       </c>
@@ -3184,8 +5031,20 @@
       <c r="F112">
         <v>110000</v>
       </c>
-    </row>
-    <row r="113" spans="1:6">
+      <c r="G112">
+        <v>14</v>
+      </c>
+      <c r="H112">
+        <v>110000</v>
+      </c>
+      <c r="I112">
+        <v>15</v>
+      </c>
+      <c r="J112" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113">
         <v>37</v>
       </c>
@@ -3204,8 +5063,20 @@
       <c r="F113">
         <v>95000</v>
       </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="G113">
+        <v>2</v>
+      </c>
+      <c r="H113">
+        <v>95000</v>
+      </c>
+      <c r="I113">
+        <v>9</v>
+      </c>
+      <c r="J113" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114">
         <v>50</v>
       </c>
@@ -3224,8 +5095,20 @@
       <c r="F114">
         <v>130000</v>
       </c>
-    </row>
-    <row r="115" spans="1:6">
+      <c r="G114">
+        <v>15</v>
+      </c>
+      <c r="H114">
+        <v>130000</v>
+      </c>
+      <c r="I114">
+        <v>22</v>
+      </c>
+      <c r="J114" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115">
         <v>32</v>
       </c>
@@ -3244,8 +5127,20 @@
       <c r="F115">
         <v>90000</v>
       </c>
-    </row>
-    <row r="116" spans="1:6">
+      <c r="G115">
+        <v>9</v>
+      </c>
+      <c r="H115">
+        <v>90000</v>
+      </c>
+      <c r="I115">
+        <v>6</v>
+      </c>
+      <c r="J115" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
       <c r="A116">
         <v>23</v>
       </c>
@@ -3264,8 +5159,20 @@
       <c r="F116">
         <v>35000</v>
       </c>
-    </row>
-    <row r="117" spans="1:6">
+      <c r="G116">
+        <v>22</v>
+      </c>
+      <c r="H116">
+        <v>35000</v>
+      </c>
+      <c r="I116">
+        <v>0.5</v>
+      </c>
+      <c r="J116" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117">
         <v>31</v>
       </c>
@@ -3284,8 +5191,20 @@
       <c r="F117">
         <v>95000</v>
       </c>
-    </row>
-    <row r="118" spans="1:6">
+      <c r="G117">
+        <v>6</v>
+      </c>
+      <c r="H117">
+        <v>95000</v>
+      </c>
+      <c r="I117">
+        <v>6</v>
+      </c>
+      <c r="J117" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
       <c r="A118">
         <v>40</v>
       </c>
@@ -3304,8 +5223,20 @@
       <c r="F118">
         <v>65000</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
+      <c r="G118">
+        <v>0.5</v>
+      </c>
+      <c r="H118">
+        <v>65000</v>
+      </c>
+      <c r="I118">
+        <v>15</v>
+      </c>
+      <c r="J118" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119">
         <v>48</v>
       </c>
@@ -3324,8 +5255,20 @@
       <c r="F119">
         <v>170000</v>
       </c>
-    </row>
-    <row r="120" spans="1:6">
+      <c r="G119">
+        <v>6</v>
+      </c>
+      <c r="H119">
+        <v>170000</v>
+      </c>
+      <c r="I119">
+        <v>20</v>
+      </c>
+      <c r="J119" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120">
         <v>29</v>
       </c>
@@ -3344,8 +5287,20 @@
       <c r="F120">
         <v>45000</v>
       </c>
-    </row>
-    <row r="121" spans="1:6">
+      <c r="G120">
+        <v>15</v>
+      </c>
+      <c r="H120">
+        <v>45000</v>
+      </c>
+      <c r="I120">
+        <v>3</v>
+      </c>
+      <c r="J120" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121">
         <v>35</v>
       </c>
@@ -3364,8 +5319,20 @@
       <c r="F121">
         <v>120000</v>
       </c>
-    </row>
-    <row r="122" spans="1:6">
+      <c r="G121">
+        <v>20</v>
+      </c>
+      <c r="H121">
+        <v>120000</v>
+      </c>
+      <c r="I121">
+        <v>10</v>
+      </c>
+      <c r="J121" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122">
         <v>42</v>
       </c>
@@ -3384,8 +5351,20 @@
       <c r="F122">
         <v>100000</v>
       </c>
-    </row>
-    <row r="123" spans="1:6">
+      <c r="G122">
+        <v>3</v>
+      </c>
+      <c r="H122">
+        <v>100000</v>
+      </c>
+      <c r="I122">
+        <v>17</v>
+      </c>
+      <c r="J122" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123">
         <v>53</v>
       </c>
@@ -3404,8 +5383,20 @@
       <c r="F123">
         <v>180000</v>
       </c>
-    </row>
-    <row r="124" spans="1:6">
+      <c r="G123">
+        <v>10</v>
+      </c>
+      <c r="H123">
+        <v>180000</v>
+      </c>
+      <c r="I123">
+        <v>25</v>
+      </c>
+      <c r="J123" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124">
         <v>33</v>
       </c>
@@ -3424,8 +5415,20 @@
       <c r="F124">
         <v>50000</v>
       </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="G124">
+        <v>17</v>
+      </c>
+      <c r="H124">
+        <v>50000</v>
+      </c>
+      <c r="I124">
+        <v>5</v>
+      </c>
+      <c r="J124" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125">
         <v>38</v>
       </c>
@@ -3444,8 +5447,20 @@
       <c r="F125">
         <v>80000</v>
       </c>
-    </row>
-    <row r="126" spans="1:6">
+      <c r="G125">
+        <v>25</v>
+      </c>
+      <c r="H125">
+        <v>80000</v>
+      </c>
+      <c r="I125">
+        <v>11</v>
+      </c>
+      <c r="J125" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
       <c r="A126">
         <v>44</v>
       </c>
@@ -3464,8 +5479,20 @@
       <c r="F126">
         <v>140000</v>
       </c>
-    </row>
-    <row r="127" spans="1:6">
+      <c r="G126">
+        <v>5</v>
+      </c>
+      <c r="H126">
+        <v>140000</v>
+      </c>
+      <c r="I126">
+        <v>16</v>
+      </c>
+      <c r="J126" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127">
         <v>26</v>
       </c>
@@ -3484,8 +5511,20 @@
       <c r="F127">
         <v>40000</v>
       </c>
-    </row>
-    <row r="128" spans="1:6">
+      <c r="G127">
+        <v>11</v>
+      </c>
+      <c r="H127">
+        <v>40000</v>
+      </c>
+      <c r="I127">
+        <v>2</v>
+      </c>
+      <c r="J127" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
       <c r="A128">
         <v>37</v>
       </c>
@@ -3504,8 +5543,20 @@
       <c r="F128">
         <v>95000</v>
       </c>
-    </row>
-    <row r="129" spans="1:6">
+      <c r="G128">
+        <v>16</v>
+      </c>
+      <c r="H128">
+        <v>95000</v>
+      </c>
+      <c r="I128">
+        <v>9</v>
+      </c>
+      <c r="J128" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
       <c r="A129">
         <v>45</v>
       </c>
@@ -3524,8 +5575,20 @@
       <c r="F129">
         <v>110000</v>
       </c>
-    </row>
-    <row r="130" spans="1:6">
+      <c r="G129">
+        <v>2</v>
+      </c>
+      <c r="H129">
+        <v>110000</v>
+      </c>
+      <c r="I129">
+        <v>18</v>
+      </c>
+      <c r="J129" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
       <c r="A130">
         <v>32</v>
       </c>
@@ -3544,8 +5607,20 @@
       <c r="F130">
         <v>50000</v>
       </c>
-    </row>
-    <row r="131" spans="1:6">
+      <c r="G130">
+        <v>9</v>
+      </c>
+      <c r="H130">
+        <v>50000</v>
+      </c>
+      <c r="I130">
+        <v>4</v>
+      </c>
+      <c r="J130" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10">
       <c r="A131">
         <v>34</v>
       </c>
@@ -3564,8 +5639,20 @@
       <c r="F131">
         <v>105000</v>
       </c>
-    </row>
-    <row r="132" spans="1:6">
+      <c r="G131">
+        <v>18</v>
+      </c>
+      <c r="H131">
+        <v>105000</v>
+      </c>
+      <c r="I131">
+        <v>8</v>
+      </c>
+      <c r="J131" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
       <c r="A132">
         <v>50</v>
       </c>
@@ -3584,8 +5671,20 @@
       <c r="F132">
         <v>160000</v>
       </c>
-    </row>
-    <row r="133" spans="1:6">
+      <c r="G132">
+        <v>4</v>
+      </c>
+      <c r="H132">
+        <v>160000</v>
+      </c>
+      <c r="I132">
+        <v>21</v>
+      </c>
+      <c r="J132" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
       <c r="A133">
         <v>29</v>
       </c>
@@ -3604,8 +5703,20 @@
       <c r="F133">
         <v>45000</v>
       </c>
-    </row>
-    <row r="134" spans="1:6">
+      <c r="G133">
+        <v>8</v>
+      </c>
+      <c r="H133">
+        <v>45000</v>
+      </c>
+      <c r="I133">
+        <v>3</v>
+      </c>
+      <c r="J133" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
       <c r="A134">
         <v>40</v>
       </c>
@@ -3624,8 +5735,20 @@
       <c r="F134">
         <v>100000</v>
       </c>
-    </row>
-    <row r="135" spans="1:6">
+      <c r="G134">
+        <v>21</v>
+      </c>
+      <c r="H134">
+        <v>100000</v>
+      </c>
+      <c r="I134">
+        <v>12</v>
+      </c>
+      <c r="J134" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
       <c r="A135">
         <v>47</v>
       </c>
@@ -3644,8 +5767,20 @@
       <c r="F135">
         <v>160000</v>
       </c>
-    </row>
-    <row r="136" spans="1:6">
+      <c r="G135">
+        <v>3</v>
+      </c>
+      <c r="H135">
+        <v>160000</v>
+      </c>
+      <c r="I135">
+        <v>22</v>
+      </c>
+      <c r="J135" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10">
       <c r="A136">
         <v>27</v>
       </c>
@@ -3664,8 +5799,20 @@
       <c r="F136">
         <v>35000</v>
       </c>
-    </row>
-    <row r="137" spans="1:6">
+      <c r="G136">
+        <v>12</v>
+      </c>
+      <c r="H136">
+        <v>35000</v>
+      </c>
+      <c r="I136">
+        <v>1</v>
+      </c>
+      <c r="J136" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10">
       <c r="A137">
         <v>39</v>
       </c>
@@ -3684,8 +5831,20 @@
       <c r="F137">
         <v>55000</v>
       </c>
-    </row>
-    <row r="138" spans="1:6">
+      <c r="G137">
+        <v>22</v>
+      </c>
+      <c r="H137">
+        <v>55000</v>
+      </c>
+      <c r="I137">
+        <v>10</v>
+      </c>
+      <c r="J137" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10">
       <c r="A138">
         <v>46</v>
       </c>
@@ -3704,8 +5863,20 @@
       <c r="F138">
         <v>140000</v>
       </c>
-    </row>
-    <row r="139" spans="1:6">
+      <c r="G138">
+        <v>1</v>
+      </c>
+      <c r="H138">
+        <v>140000</v>
+      </c>
+      <c r="I138">
+        <v>19</v>
+      </c>
+      <c r="J138" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
       <c r="A139">
         <v>30</v>
       </c>
@@ -3724,8 +5895,20 @@
       <c r="F139">
         <v>50000</v>
       </c>
-    </row>
-    <row r="140" spans="1:6">
+      <c r="G139">
+        <v>10</v>
+      </c>
+      <c r="H139">
+        <v>50000</v>
+      </c>
+      <c r="I139">
+        <v>4</v>
+      </c>
+      <c r="J139" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
       <c r="A140">
         <v>36</v>
       </c>
@@ -3744,8 +5927,20 @@
       <c r="F140">
         <v>60000</v>
       </c>
-    </row>
-    <row r="141" spans="1:6">
+      <c r="G140">
+        <v>19</v>
+      </c>
+      <c r="H140">
+        <v>60000</v>
+      </c>
+      <c r="I140">
+        <v>7</v>
+      </c>
+      <c r="J140" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
       <c r="A141">
         <v>43</v>
       </c>
@@ -3764,8 +5959,20 @@
       <c r="F141">
         <v>120000</v>
       </c>
-    </row>
-    <row r="142" spans="1:6">
+      <c r="G141">
+        <v>4</v>
+      </c>
+      <c r="H141">
+        <v>120000</v>
+      </c>
+      <c r="I141">
+        <v>14</v>
+      </c>
+      <c r="J141" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10">
       <c r="A142">
         <v>28</v>
       </c>
@@ -3784,8 +5991,20 @@
       <c r="F142">
         <v>40000</v>
       </c>
-    </row>
-    <row r="143" spans="1:6">
+      <c r="G142">
+        <v>7</v>
+      </c>
+      <c r="H142">
+        <v>40000</v>
+      </c>
+      <c r="I142">
+        <v>2</v>
+      </c>
+      <c r="J142" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
       <c r="A143">
         <v>41</v>
       </c>
@@ -3804,8 +6023,20 @@
       <c r="F143">
         <v>110000</v>
       </c>
-    </row>
-    <row r="144" spans="1:6">
+      <c r="G143">
+        <v>14</v>
+      </c>
+      <c r="H143">
+        <v>110000</v>
+      </c>
+      <c r="I143">
+        <v>13</v>
+      </c>
+      <c r="J143" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
       <c r="A144">
         <v>33</v>
       </c>
@@ -3824,8 +6055,20 @@
       <c r="F144">
         <v>50000</v>
       </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="G144">
+        <v>2</v>
+      </c>
+      <c r="H144">
+        <v>50000</v>
+      </c>
+      <c r="I144">
+        <v>5</v>
+      </c>
+      <c r="J144" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
       <c r="A145">
         <v>47</v>
       </c>
@@ -3844,8 +6087,20 @@
       <c r="F145">
         <v>135000</v>
       </c>
-    </row>
-    <row r="146" spans="1:6">
+      <c r="G145">
+        <v>13</v>
+      </c>
+      <c r="H145">
+        <v>135000</v>
+      </c>
+      <c r="I145">
+        <v>20</v>
+      </c>
+      <c r="J145" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
       <c r="A146">
         <v>25</v>
       </c>
@@ -3864,8 +6119,20 @@
       <c r="F146">
         <v>40000</v>
       </c>
-    </row>
-    <row r="147" spans="1:6">
+      <c r="G146">
+        <v>5</v>
+      </c>
+      <c r="H146">
+        <v>40000</v>
+      </c>
+      <c r="I146">
+        <v>1.5</v>
+      </c>
+      <c r="J146" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
       <c r="A147">
         <v>34</v>
       </c>
@@ -3884,8 +6151,20 @@
       <c r="F147">
         <v>90000</v>
       </c>
-    </row>
-    <row r="148" spans="1:6">
+      <c r="G147">
+        <v>20</v>
+      </c>
+      <c r="H147">
+        <v>90000</v>
+      </c>
+      <c r="I147">
+        <v>8</v>
+      </c>
+      <c r="J147" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10">
       <c r="A148">
         <v>42</v>
       </c>
@@ -3904,8 +6183,20 @@
       <c r="F148">
         <v>150000</v>
       </c>
-    </row>
-    <row r="149" spans="1:6">
+      <c r="G148">
+        <v>1.5</v>
+      </c>
+      <c r="H148">
+        <v>150000</v>
+      </c>
+      <c r="I148">
+        <v>16</v>
+      </c>
+      <c r="J148" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10">
       <c r="A149">
         <v>31</v>
       </c>
@@ -3924,8 +6215,20 @@
       <c r="F149">
         <v>60000</v>
       </c>
-    </row>
-    <row r="150" spans="1:6">
+      <c r="G149">
+        <v>8</v>
+      </c>
+      <c r="H149">
+        <v>60000</v>
+      </c>
+      <c r="I149">
+        <v>4</v>
+      </c>
+      <c r="J149" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
       <c r="A150">
         <v>38</v>
       </c>
@@ -3944,8 +6247,20 @@
       <c r="F150">
         <v>80000</v>
       </c>
-    </row>
-    <row r="151" spans="1:6">
+      <c r="G150">
+        <v>16</v>
+      </c>
+      <c r="H150">
+        <v>80000</v>
+      </c>
+      <c r="I150">
+        <v>10</v>
+      </c>
+      <c r="J150" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10">
       <c r="A151">
         <v>45</v>
       </c>
@@ -3964,8 +6279,20 @@
       <c r="F151">
         <v>175000</v>
       </c>
-    </row>
-    <row r="152" spans="1:6">
+      <c r="G151">
+        <v>4</v>
+      </c>
+      <c r="H151">
+        <v>175000</v>
+      </c>
+      <c r="I151">
+        <v>19</v>
+      </c>
+      <c r="J151" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10">
       <c r="A152">
         <v>29</v>
       </c>
@@ -3984,8 +6311,20 @@
       <c r="F152">
         <v>45000</v>
       </c>
-    </row>
-    <row r="153" spans="1:6">
+      <c r="G152">
+        <v>10</v>
+      </c>
+      <c r="H152">
+        <v>45000</v>
+      </c>
+      <c r="I152">
+        <v>3</v>
+      </c>
+      <c r="J152" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
       <c r="A153">
         <v>36</v>
       </c>
@@ -4004,8 +6343,20 @@
       <c r="F153">
         <v>120000</v>
       </c>
-    </row>
-    <row r="154" spans="1:6">
+      <c r="G153">
+        <v>19</v>
+      </c>
+      <c r="H153">
+        <v>120000</v>
+      </c>
+      <c r="I153">
+        <v>11</v>
+      </c>
+      <c r="J153" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10">
       <c r="A154">
         <v>43</v>
       </c>
@@ -4024,8 +6375,20 @@
       <c r="F154">
         <v>140000</v>
       </c>
-    </row>
-    <row r="155" spans="1:6">
+      <c r="G154">
+        <v>3</v>
+      </c>
+      <c r="H154">
+        <v>140000</v>
+      </c>
+      <c r="I154">
+        <v>18</v>
+      </c>
+      <c r="J154" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
       <c r="A155">
         <v>26</v>
       </c>
@@ -4044,8 +6407,20 @@
       <c r="F155">
         <v>35000</v>
       </c>
-    </row>
-    <row r="156" spans="1:6">
+      <c r="G155">
+        <v>11</v>
+      </c>
+      <c r="H155">
+        <v>35000</v>
+      </c>
+      <c r="I155">
+        <v>2</v>
+      </c>
+      <c r="J155" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
       <c r="A156">
         <v>37</v>
       </c>
@@ -4064,8 +6439,20 @@
       <c r="F156">
         <v>95000</v>
       </c>
-    </row>
-    <row r="157" spans="1:6">
+      <c r="G156">
+        <v>18</v>
+      </c>
+      <c r="H156">
+        <v>95000</v>
+      </c>
+      <c r="I156">
+        <v>9</v>
+      </c>
+      <c r="J156" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10">
       <c r="A157">
         <v>44</v>
       </c>
@@ -4084,8 +6471,20 @@
       <c r="F157">
         <v>110000</v>
       </c>
-    </row>
-    <row r="158" spans="1:6">
+      <c r="G157">
+        <v>2</v>
+      </c>
+      <c r="H157">
+        <v>110000</v>
+      </c>
+      <c r="I157">
+        <v>14</v>
+      </c>
+      <c r="J157" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10">
       <c r="A158">
         <v>32</v>
       </c>
@@ -4104,8 +6503,20 @@
       <c r="F158">
         <v>50000</v>
       </c>
-    </row>
-    <row r="159" spans="1:6">
+      <c r="G158">
+        <v>9</v>
+      </c>
+      <c r="H158">
+        <v>50000</v>
+      </c>
+      <c r="I158">
+        <v>5</v>
+      </c>
+      <c r="J158" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10">
       <c r="A159">
         <v>33</v>
       </c>
@@ -4124,8 +6535,20 @@
       <c r="F159">
         <v>115000</v>
       </c>
-    </row>
-    <row r="160" spans="1:6">
+      <c r="G159">
+        <v>14</v>
+      </c>
+      <c r="H159">
+        <v>115000</v>
+      </c>
+      <c r="I159">
+        <v>7</v>
+      </c>
+      <c r="J159" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10">
       <c r="A160">
         <v>51</v>
       </c>
@@ -4144,8 +6567,20 @@
       <c r="F160">
         <v>185000</v>
       </c>
-    </row>
-    <row r="161" spans="1:6">
+      <c r="G160">
+        <v>5</v>
+      </c>
+      <c r="H160">
+        <v>185000</v>
+      </c>
+      <c r="I160">
+        <v>23</v>
+      </c>
+      <c r="J160" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10">
       <c r="A161">
         <v>28</v>
       </c>
@@ -4164,8 +6599,20 @@
       <c r="F161">
         <v>40000</v>
       </c>
-    </row>
-    <row r="162" spans="1:6">
+      <c r="G161">
+        <v>7</v>
+      </c>
+      <c r="H161">
+        <v>40000</v>
+      </c>
+      <c r="I161">
+        <v>2</v>
+      </c>
+      <c r="J161" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10">
       <c r="A162">
         <v>39</v>
       </c>
@@ -4184,8 +6631,20 @@
       <c r="F162">
         <v>90000</v>
       </c>
-    </row>
-    <row r="163" spans="1:6">
+      <c r="G162">
+        <v>23</v>
+      </c>
+      <c r="H162">
+        <v>90000</v>
+      </c>
+      <c r="I162">
+        <v>12</v>
+      </c>
+      <c r="J162" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10">
       <c r="A163">
         <v>48</v>
       </c>
@@ -4204,8 +6663,20 @@
       <c r="F163">
         <v>175000</v>
       </c>
-    </row>
-    <row r="164" spans="1:6">
+      <c r="G163">
+        <v>2</v>
+      </c>
+      <c r="H163">
+        <v>175000</v>
+      </c>
+      <c r="I163">
+        <v>21</v>
+      </c>
+      <c r="J163" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10">
       <c r="A164">
         <v>30</v>
       </c>
@@ -4224,8 +6695,20 @@
       <c r="F164">
         <v>45000</v>
       </c>
-    </row>
-    <row r="165" spans="1:6">
+      <c r="G164">
+        <v>12</v>
+      </c>
+      <c r="H164">
+        <v>45000</v>
+      </c>
+      <c r="I164">
+        <v>3</v>
+      </c>
+      <c r="J164" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10">
       <c r="A165">
         <v>35</v>
       </c>
@@ -4244,8 +6727,20 @@
       <c r="F165">
         <v>80000</v>
       </c>
-    </row>
-    <row r="166" spans="1:6">
+      <c r="G165">
+        <v>21</v>
+      </c>
+      <c r="H165">
+        <v>80000</v>
+      </c>
+      <c r="I165">
+        <v>7</v>
+      </c>
+      <c r="J165" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10">
       <c r="A166">
         <v>41</v>
       </c>
@@ -4264,8 +6759,20 @@
       <c r="F166">
         <v>120000</v>
       </c>
-    </row>
-    <row r="167" spans="1:6">
+      <c r="G166">
+        <v>3</v>
+      </c>
+      <c r="H166">
+        <v>120000</v>
+      </c>
+      <c r="I166">
+        <v>13</v>
+      </c>
+      <c r="J166" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10">
       <c r="A167">
         <v>27</v>
       </c>
@@ -4284,8 +6791,20 @@
       <c r="F167">
         <v>35000</v>
       </c>
-    </row>
-    <row r="168" spans="1:6">
+      <c r="G167">
+        <v>7</v>
+      </c>
+      <c r="H167">
+        <v>35000</v>
+      </c>
+      <c r="I167">
+        <v>1.5</v>
+      </c>
+      <c r="J167" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10">
       <c r="A168">
         <v>40</v>
       </c>
@@ -4304,8 +6823,20 @@
       <c r="F168">
         <v>110000</v>
       </c>
-    </row>
-    <row r="169" spans="1:6">
+      <c r="G168">
+        <v>13</v>
+      </c>
+      <c r="H168">
+        <v>110000</v>
+      </c>
+      <c r="I168">
+        <v>14</v>
+      </c>
+      <c r="J168" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10">
       <c r="A169">
         <v>46</v>
       </c>
@@ -4324,8 +6855,20 @@
       <c r="F169">
         <v>150000</v>
       </c>
-    </row>
-    <row r="170" spans="1:6">
+      <c r="G169">
+        <v>1.5</v>
+      </c>
+      <c r="H169">
+        <v>150000</v>
+      </c>
+      <c r="I169">
+        <v>18</v>
+      </c>
+      <c r="J169" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10">
       <c r="A170">
         <v>31</v>
       </c>
@@ -4344,8 +6887,20 @@
       <c r="F170">
         <v>50000</v>
       </c>
-    </row>
-    <row r="171" spans="1:6">
+      <c r="G170">
+        <v>14</v>
+      </c>
+      <c r="H170">
+        <v>50000</v>
+      </c>
+      <c r="I170">
+        <v>4</v>
+      </c>
+      <c r="J170" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10">
       <c r="A171">
         <v>34</v>
       </c>
@@ -4364,8 +6919,20 @@
       <c r="F171">
         <v>105000</v>
       </c>
-    </row>
-    <row r="172" spans="1:6">
+      <c r="G171">
+        <v>18</v>
+      </c>
+      <c r="H171">
+        <v>105000</v>
+      </c>
+      <c r="I171">
+        <v>9</v>
+      </c>
+      <c r="J171" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10">
       <c r="A172">
         <v>50</v>
       </c>
@@ -4384,8 +6951,20 @@
       <c r="F172">
         <v>180000</v>
       </c>
-    </row>
-    <row r="173" spans="1:6">
+      <c r="G172">
+        <v>4</v>
+      </c>
+      <c r="H172">
+        <v>180000</v>
+      </c>
+      <c r="I172">
+        <v>20</v>
+      </c>
+      <c r="J172" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10">
       <c r="A173">
         <v>29</v>
       </c>
@@ -4404,9 +6983,23 @@
       <c r="F173">
         <v>40000</v>
       </c>
+      <c r="G173">
+        <v>9</v>
+      </c>
+      <c r="H173">
+        <v>40000</v>
+      </c>
+      <c r="I173">
+        <v>2</v>
+      </c>
+      <c r="J173" t="s">
+        <v>327</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4418,7 +7011,7 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">

</xml_diff>